<commit_message>
use lstm for all item
</commit_message>
<xml_diff>
--- a/public/assets/sample-stock-import.xlsx
+++ b/public/assets/sample-stock-import.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3577AC-0807-4CC6-9738-5BA2F09F67BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C376D1-B4AE-47EC-ACDD-018A2673EABE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14400" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>SKU</t>
   </si>
@@ -34,40 +34,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Sed quia sunt dolor quis similique deleniti quas.</t>
-  </si>
-  <si>
-    <t>Voluptatum quis vero maxime numquam quibusdam dolorum ad.</t>
-  </si>
-  <si>
-    <t>Enim odio aliquam minima voluptatem sit incidunt.</t>
-  </si>
-  <si>
-    <t>Beatae corrupti id eum consequatur voluptatem.</t>
-  </si>
-  <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>PCS</t>
-  </si>
-  <si>
-    <t>O50AF40I</t>
-  </si>
-  <si>
-    <t>A15VPBJA</t>
-  </si>
-  <si>
-    <t>4LKBTXSW</t>
-  </si>
-  <si>
-    <t>NGODJUGJ</t>
   </si>
 </sst>
 </file>
@@ -103,7 +70,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,27 +93,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -429,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,76 +408,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2">
-        <v>78</v>
-      </c>
-      <c r="D2">
-        <v>176.54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>279.56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>405.69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>58.25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>